<commit_message>
Debuged the code. 8 hours generator still not working properly, shiould be checked.
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Legolas\Desktop\schedule-generator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="schedule" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="emails" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="schedule" sheetId="2" r:id="rId2"/>
+    <sheet name="emails" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,455 +28,452 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="147">
   <si>
-    <t xml:space="preserve">January '21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basaria Daviti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS4/SS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devi Devidze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SS/FS4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cherkezishvili Tornike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shiukashvili Mariana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nakopia Ana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mtvarelishvili Nika</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zurab Maisaia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kutubidze Diana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Velijanashvili Tamta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nana Amoevi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drozdova Tamar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anana Ananiashvili</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gelovani Nodar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shamatava Mamuka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New FS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Todua Zaza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gvatua Eka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imnadze Ani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arachemia Nino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regina Kruger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ackasova Aleksandra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sulaberidze Nino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giorgi Maisuradze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chkheidze Nino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Makhatadze Davit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beniashvili Victoria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marina Romanovskaia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siradze Sopiko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Razmadze Niko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imamaliyev Yagub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bachoshvili Giorgi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Artemi Arutinovi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khardziani Tamari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ioseliani Anastasia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kudzoshvili Teona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kandelaki Tsira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chincharauli Giga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tskhvedadze Sandro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petriashvili Tornike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chapidze Natalia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Savaneli Nino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dartsmelia Mamuka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Razmadze Natia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tsomaia Tinatin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ekaterine Kartsivadze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ismailov Idaiat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elyar Akhi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tevzadze Ilia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nairashvili Elene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utiashvili Tamar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kadzanaia Tamar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isaev Muraz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rukhaia Nana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erkut Batuhan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kama Mustafa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magalashvili Lala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kvaratskhelia Marika</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gogoberishvili Aleksandre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kikaleishvili Ana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nanitashvili Revaz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maisaia Zurab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amoevi Nana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ananiashvili Anana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kruger Regina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maisuradze Giorgi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Romanovskaia Marina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arutinovi Artemi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kartsivadze Ekaterine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emails</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aackasova@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aananiashvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aarutinovi@evolution.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aelyar@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">agogoberishvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aimnadze@evolution.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aioseliani@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">akikaleishvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anakopia@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">berkut@evolution.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve">dbasaria@evolutiongaming.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ddevidze@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dkutubidze@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dmakhatadze@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">egvatua@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ekartsivadze@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enairashvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gbachoshvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gchincharauli@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gmaisuradze@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iismailovi@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">itevzadze@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lmagalashvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mdartsmelia@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">misaev@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mkama@evolution.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mkvaratskhelia3@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mromanovskaia@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mshamatava@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mshiukashvili@evolution.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve">namoevi@evolution.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve">narachemia@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nchapidze@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nchkheidze@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ngelovani@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nmtvarelishvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nrazmadze3@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nrazmadze5@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nrukhaia@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nsavaneli@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nsulaberidze@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rkruger@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rnanitashvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssiradze@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stskhvedadze@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tcherkezishvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tdrozdova@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tkadzanaia@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tkandelaki@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tkhardziani@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tkudzoshvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tpetriashvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ttsomaia@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tutiashvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tvelijanashvili@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vbeniashvili@evolution.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yimamaliyev@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zmaisaia@evolution.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztodua@evolution.com</t>
+    <t>January '21</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Tu</t>
+  </si>
+  <si>
+    <t>We</t>
+  </si>
+  <si>
+    <t>Th</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Sat</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>SET</t>
+  </si>
+  <si>
+    <t>Basaria Daviti</t>
+  </si>
+  <si>
+    <t>FS6</t>
+  </si>
+  <si>
+    <t>FS5</t>
+  </si>
+  <si>
+    <t>Vac</t>
+  </si>
+  <si>
+    <t>FS4/SS</t>
+  </si>
+  <si>
+    <t>FS1</t>
+  </si>
+  <si>
+    <t>FS2</t>
+  </si>
+  <si>
+    <t>Devi Devidze</t>
+  </si>
+  <si>
+    <t>SS/FS4</t>
+  </si>
+  <si>
+    <t>FS7</t>
+  </si>
+  <si>
+    <t>Cherkezishvili Tornike</t>
+  </si>
+  <si>
+    <t>FS3</t>
+  </si>
+  <si>
+    <t>Shiukashvili Mariana</t>
+  </si>
+  <si>
+    <t>Nakopia Ana</t>
+  </si>
+  <si>
+    <t>Mtvarelishvili Nika</t>
+  </si>
+  <si>
+    <t>Zurab Maisaia</t>
+  </si>
+  <si>
+    <t>Kutubidze Diana</t>
+  </si>
+  <si>
+    <t>Velijanashvili Tamta</t>
+  </si>
+  <si>
+    <t>Nana Amoevi</t>
+  </si>
+  <si>
+    <t>Drozdova Tamar</t>
+  </si>
+  <si>
+    <t>Anana Ananiashvili</t>
+  </si>
+  <si>
+    <t>Gelovani Nodar</t>
+  </si>
+  <si>
+    <t>Shamatava Mamuka</t>
+  </si>
+  <si>
+    <t>New FS</t>
+  </si>
+  <si>
+    <t>Todua Zaza</t>
+  </si>
+  <si>
+    <t>Gvatua Eka</t>
+  </si>
+  <si>
+    <t>Imnadze Ani</t>
+  </si>
+  <si>
+    <t>Arachemia Nino</t>
+  </si>
+  <si>
+    <t>Regina Kruger</t>
+  </si>
+  <si>
+    <t>Ackasova Aleksandra</t>
+  </si>
+  <si>
+    <t>Sulaberidze Nino</t>
+  </si>
+  <si>
+    <t>Giorgi Maisuradze</t>
+  </si>
+  <si>
+    <t>Chkheidze Nino</t>
+  </si>
+  <si>
+    <t>Makhatadze Davit</t>
+  </si>
+  <si>
+    <t>Beniashvili Victoria</t>
+  </si>
+  <si>
+    <t>Marina Romanovskaia</t>
+  </si>
+  <si>
+    <t>Siradze Sopiko</t>
+  </si>
+  <si>
+    <t>Razmadze Niko</t>
+  </si>
+  <si>
+    <t>Imamaliyev Yagub</t>
+  </si>
+  <si>
+    <t>Bachoshvili Giorgi</t>
+  </si>
+  <si>
+    <t>GAPS</t>
+  </si>
+  <si>
+    <t>Artemi Arutinovi</t>
+  </si>
+  <si>
+    <t>Khardziani Tamari</t>
+  </si>
+  <si>
+    <t>Ioseliani Anastasia</t>
+  </si>
+  <si>
+    <t>Kudzoshvili Teona</t>
+  </si>
+  <si>
+    <t>Kandelaki Tsira</t>
+  </si>
+  <si>
+    <t>Chincharauli Giga</t>
+  </si>
+  <si>
+    <t>Tskhvedadze Sandro</t>
+  </si>
+  <si>
+    <t>Petriashvili Tornike</t>
+  </si>
+  <si>
+    <t>Chapidze Natalia</t>
+  </si>
+  <si>
+    <t>Savaneli Nino</t>
+  </si>
+  <si>
+    <t>Dartsmelia Mamuka</t>
+  </si>
+  <si>
+    <t>Razmadze Natia</t>
+  </si>
+  <si>
+    <t>Tsomaia Tinatin</t>
+  </si>
+  <si>
+    <t>Ekaterine Kartsivadze</t>
+  </si>
+  <si>
+    <t>Ismailov Idaiat</t>
+  </si>
+  <si>
+    <t>Elyar Akhi</t>
+  </si>
+  <si>
+    <t>Tevzadze Ilia</t>
+  </si>
+  <si>
+    <t>Nairashvili Elene</t>
+  </si>
+  <si>
+    <t>Utiashvili Tamar</t>
+  </si>
+  <si>
+    <t>Kadzanaia Tamar</t>
+  </si>
+  <si>
+    <t>Isaev Muraz</t>
+  </si>
+  <si>
+    <t>Rukhaia Nana</t>
+  </si>
+  <si>
+    <t>Erkut Batuhan</t>
+  </si>
+  <si>
+    <t>Kama Mustafa</t>
+  </si>
+  <si>
+    <t>Magalashvili Lala</t>
+  </si>
+  <si>
+    <t>Kvaratskhelia Marika</t>
+  </si>
+  <si>
+    <t>Gogoberishvili Aleksandre</t>
+  </si>
+  <si>
+    <t>Kikaleishvili Ana</t>
+  </si>
+  <si>
+    <t>Nanitashvili Revaz</t>
+  </si>
+  <si>
+    <t>Maisaia Zurab</t>
+  </si>
+  <si>
+    <t>Amoevi Nana</t>
+  </si>
+  <si>
+    <t>Ananiashvili Anana</t>
+  </si>
+  <si>
+    <t>Kruger Regina</t>
+  </si>
+  <si>
+    <t>Maisuradze Giorgi</t>
+  </si>
+  <si>
+    <t>Romanovskaia Marina</t>
+  </si>
+  <si>
+    <t>Arutinovi Artemi</t>
+  </si>
+  <si>
+    <t>Kartsivadze Ekaterine</t>
+  </si>
+  <si>
+    <t>emails</t>
+  </si>
+  <si>
+    <t>aackasova@evolution.com</t>
+  </si>
+  <si>
+    <t>aananiashvili@evolution.com</t>
+  </si>
+  <si>
+    <t>aarutinovi@evolution.com </t>
+  </si>
+  <si>
+    <t>aelyar@evolution.com</t>
+  </si>
+  <si>
+    <t>agogoberishvili@evolution.com</t>
+  </si>
+  <si>
+    <t>aimnadze@evolution.com </t>
+  </si>
+  <si>
+    <t>aioseliani@evolution.com</t>
+  </si>
+  <si>
+    <t>akikaleishvili@evolution.com</t>
+  </si>
+  <si>
+    <t>anakopia@evolution.com</t>
+  </si>
+  <si>
+    <t>berkut@evolution.com </t>
+  </si>
+  <si>
+    <t>dbasaria@evolutiongaming.com</t>
+  </si>
+  <si>
+    <t>ddevidze@evolution.com</t>
+  </si>
+  <si>
+    <t>dkutubidze@evolution.com</t>
+  </si>
+  <si>
+    <t>dmakhatadze@evolution.com</t>
+  </si>
+  <si>
+    <t>egvatua@evolution.com</t>
+  </si>
+  <si>
+    <t>ekartsivadze@evolution.com</t>
+  </si>
+  <si>
+    <t>enairashvili@evolution.com</t>
+  </si>
+  <si>
+    <t>gbachoshvili@evolution.com</t>
+  </si>
+  <si>
+    <t>gchincharauli@evolution.com</t>
+  </si>
+  <si>
+    <t>gmaisuradze@evolution.com</t>
+  </si>
+  <si>
+    <t>iismailovi@evolution.com</t>
+  </si>
+  <si>
+    <t>itevzadze@evolution.com</t>
+  </si>
+  <si>
+    <t>lmagalashvili@evolution.com</t>
+  </si>
+  <si>
+    <t>Mdartsmelia@evolution.com</t>
+  </si>
+  <si>
+    <t>misaev@evolution.com</t>
+  </si>
+  <si>
+    <t>mkama@evolution.com </t>
+  </si>
+  <si>
+    <t>Mkvaratskhelia3@evolution.com</t>
+  </si>
+  <si>
+    <t>mromanovskaia@evolution.com</t>
+  </si>
+  <si>
+    <t>mshamatava@evolution.com</t>
+  </si>
+  <si>
+    <t>mshiukashvili@evolution.com </t>
+  </si>
+  <si>
+    <t>namoevi@evolution.com </t>
+  </si>
+  <si>
+    <t>narachemia@evolution.com</t>
+  </si>
+  <si>
+    <t>nchapidze@evolution.com</t>
+  </si>
+  <si>
+    <t>nchkheidze@evolution.com</t>
+  </si>
+  <si>
+    <t>ngelovani@evolution.com</t>
+  </si>
+  <si>
+    <t>nmtvarelishvili@evolution.com</t>
+  </si>
+  <si>
+    <t>nrazmadze3@evolution.com</t>
+  </si>
+  <si>
+    <t>nrazmadze5@evolution.com</t>
+  </si>
+  <si>
+    <t>nrukhaia@evolution.com</t>
+  </si>
+  <si>
+    <t>nsavaneli@evolution.com</t>
+  </si>
+  <si>
+    <t>nsulaberidze@evolution.com</t>
+  </si>
+  <si>
+    <t>rkruger@evolution.com</t>
+  </si>
+  <si>
+    <t>rnanitashvili@evolution.com</t>
+  </si>
+  <si>
+    <t>ssiradze@evolution.com</t>
+  </si>
+  <si>
+    <t>stskhvedadze@evolution.com</t>
+  </si>
+  <si>
+    <t>tcherkezishvili@evolution.com</t>
+  </si>
+  <si>
+    <t>tdrozdova@evolution.com</t>
+  </si>
+  <si>
+    <t>tkadzanaia@evolution.com</t>
+  </si>
+  <si>
+    <t>tkandelaki@evolution.com</t>
+  </si>
+  <si>
+    <t>tkhardziani@evolution.com</t>
+  </si>
+  <si>
+    <t>tkudzoshvili@evolution.com</t>
+  </si>
+  <si>
+    <t>tpetriashvili@evolution.com</t>
+  </si>
+  <si>
+    <t>ttsomaia@evolution.com</t>
+  </si>
+  <si>
+    <t>tutiashvili@evolution.com</t>
+  </si>
+  <si>
+    <t>tvelijanashvili@evolution.com</t>
+  </si>
+  <si>
+    <t>vbeniashvili@evolution.com </t>
+  </si>
+  <si>
+    <t>yimamaliyev@evolution.com</t>
+  </si>
+  <si>
+    <t>zmaisaia@evolution.com</t>
+  </si>
+  <si>
+    <t>ztodua@evolution.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -481,22 +482,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
@@ -504,7 +490,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,186 +551,139 @@
         <bgColor rgb="FFE2F0D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FF9DC3E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFE2F0D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF9DC3E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFE2F0D9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="34">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -788,6 +727,7 @@
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -846,28 +786,302 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+  <a:themeElements>
+    <a:clrScheme name="Стандартная">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Стандартная">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Стандартная">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.71"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -957,101 +1171,101 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="3">
         <v>1.2</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="E2" s="3" t="n">
+      <c r="D2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E2" s="3">
         <v>3.2</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="1">
         <v>4.2</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="1">
         <v>5.2</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>6.2</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="3">
         <v>7.2</v>
       </c>
-      <c r="J2" s="3" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="K2" s="3" t="n">
-        <v>9.2</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>10.2</v>
-      </c>
-      <c r="M2" s="1" t="n">
+      <c r="J2" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K2" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M2" s="1">
         <v>11.2</v>
       </c>
-      <c r="N2" s="1" t="n">
+      <c r="N2" s="1">
         <v>12.2</v>
       </c>
-      <c r="O2" s="3" t="n">
+      <c r="O2" s="3">
         <v>13.2</v>
       </c>
-      <c r="P2" s="3" t="n">
+      <c r="P2" s="3">
         <v>14.2</v>
       </c>
-      <c r="Q2" s="3" t="n">
+      <c r="Q2" s="3">
         <v>15.2</v>
       </c>
-      <c r="R2" s="1" t="n">
+      <c r="R2" s="1">
         <v>16.2</v>
       </c>
-      <c r="S2" s="1" t="n">
+      <c r="S2" s="1">
         <v>17.2</v>
       </c>
-      <c r="T2" s="1" t="n">
+      <c r="T2" s="1">
         <v>18.2</v>
       </c>
-      <c r="U2" s="3" t="n">
+      <c r="U2" s="3">
         <v>19.2</v>
       </c>
-      <c r="V2" s="3" t="n">
+      <c r="V2" s="3">
         <v>20.2</v>
       </c>
-      <c r="W2" s="3" t="n">
+      <c r="W2" s="3">
         <v>21.2</v>
       </c>
-      <c r="X2" s="1" t="n">
+      <c r="X2" s="1">
         <v>22.2</v>
       </c>
-      <c r="Y2" s="1" t="n">
+      <c r="Y2" s="1">
         <v>23.2</v>
       </c>
-      <c r="Z2" s="1" t="n">
+      <c r="Z2" s="1">
         <v>24.2</v>
       </c>
-      <c r="AA2" s="3" t="n">
+      <c r="AA2" s="3">
         <v>25.2</v>
       </c>
-      <c r="AB2" s="3" t="n">
+      <c r="AB2" s="3">
         <v>26.2</v>
       </c>
-      <c r="AC2" s="3" t="n">
+      <c r="AC2" s="3">
         <v>27.2</v>
       </c>
-      <c r="AD2" s="1" t="n">
+      <c r="AD2" s="1">
         <v>28.2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1109,11 +1323,11 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
@@ -1161,11 +1375,11 @@
       </c>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1"/>
@@ -1211,11 +1425,11 @@
       </c>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1261,11 +1475,11 @@
       </c>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1311,11 +1525,11 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1371,11 +1585,11 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1431,11 +1645,11 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="8"/>
@@ -1481,11 +1695,11 @@
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1543,11 +1757,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1595,11 +1809,11 @@
       </c>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1"/>
@@ -1647,11 +1861,11 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1715,11 +1929,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1767,11 +1981,11 @@
       </c>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1"/>
@@ -1817,11 +2031,11 @@
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="10" t="n">
+      <c r="B17" s="10">
         <v>1</v>
       </c>
       <c r="C17" s="11"/>
@@ -1865,11 +2079,11 @@
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="10" t="n">
+      <c r="B18" s="10">
         <v>1</v>
       </c>
       <c r="C18" s="11"/>
@@ -1913,11 +2127,11 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="13" t="n">
+      <c r="B19" s="13">
         <v>1</v>
       </c>
       <c r="C19" s="13"/>
@@ -1981,11 +2195,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="7" t="n">
+      <c r="B20" s="7">
         <v>2</v>
       </c>
       <c r="C20" s="7"/>
@@ -2029,11 +2243,11 @@
       <c r="AC20" s="7"/>
       <c r="AD20" s="7"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="1">
         <v>2</v>
       </c>
       <c r="C21" s="8"/>
@@ -2077,11 +2291,11 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="1">
         <v>2</v>
       </c>
       <c r="C22" s="8"/>
@@ -2137,11 +2351,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="B23" s="1">
         <v>2</v>
       </c>
       <c r="C23" s="8"/>
@@ -2185,11 +2399,11 @@
       <c r="AC23" s="7"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" s="1">
         <v>2</v>
       </c>
       <c r="C24" s="19"/>
@@ -2233,11 +2447,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="8"/>
@@ -2283,11 +2497,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" s="1">
         <v>2</v>
       </c>
       <c r="C26" s="1"/>
@@ -2343,11 +2557,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="1">
         <v>2</v>
       </c>
       <c r="C27" s="1"/>
@@ -2393,11 +2607,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="1">
         <v>2</v>
       </c>
       <c r="C28" s="1"/>
@@ -2443,11 +2657,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="1">
         <v>2</v>
       </c>
       <c r="C29" s="1"/>
@@ -2493,11 +2707,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="1">
         <v>2</v>
       </c>
       <c r="C30" s="1"/>
@@ -2553,11 +2767,11 @@
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="1">
         <v>2</v>
       </c>
       <c r="C31" s="1"/>
@@ -2623,11 +2837,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="1">
         <v>2</v>
       </c>
       <c r="C32" s="1"/>
@@ -2673,11 +2887,11 @@
       </c>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="1">
         <v>2</v>
       </c>
       <c r="C33" s="1"/>
@@ -2733,11 +2947,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="1">
         <v>2</v>
       </c>
       <c r="C34" s="1"/>
@@ -2781,11 +2995,11 @@
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="1">
         <v>2</v>
       </c>
       <c r="C35" s="1"/>
@@ -2851,7 +3065,7 @@
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
@@ -2885,7 +3099,7 @@
       <c r="AC36" s="20"/>
       <c r="AD36" s="20"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -2975,101 +3189,101 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" s="3">
         <v>1.2</v>
       </c>
-      <c r="D38" s="3" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="E38" s="3" t="n">
+      <c r="D38" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E38" s="3">
         <v>3.2</v>
       </c>
-      <c r="F38" s="1" t="n">
+      <c r="F38" s="1">
         <v>4.2</v>
       </c>
-      <c r="G38" s="1" t="n">
+      <c r="G38" s="1">
         <v>5.2</v>
       </c>
-      <c r="H38" s="1" t="n">
+      <c r="H38" s="1">
         <v>6.2</v>
       </c>
-      <c r="I38" s="3" t="n">
+      <c r="I38" s="3">
         <v>7.2</v>
       </c>
-      <c r="J38" s="3" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="K38" s="3" t="n">
-        <v>9.2</v>
-      </c>
-      <c r="L38" s="1" t="n">
-        <v>10.2</v>
-      </c>
-      <c r="M38" s="1" t="n">
+      <c r="J38" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K38" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L38" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M38" s="1">
         <v>11.2</v>
       </c>
-      <c r="N38" s="1" t="n">
+      <c r="N38" s="1">
         <v>12.2</v>
       </c>
-      <c r="O38" s="3" t="n">
+      <c r="O38" s="3">
         <v>13.2</v>
       </c>
-      <c r="P38" s="3" t="n">
+      <c r="P38" s="3">
         <v>14.2</v>
       </c>
-      <c r="Q38" s="3" t="n">
+      <c r="Q38" s="3">
         <v>15.2</v>
       </c>
-      <c r="R38" s="1" t="n">
+      <c r="R38" s="1">
         <v>16.2</v>
       </c>
-      <c r="S38" s="1" t="n">
+      <c r="S38" s="1">
         <v>17.2</v>
       </c>
-      <c r="T38" s="1" t="n">
+      <c r="T38" s="1">
         <v>18.2</v>
       </c>
-      <c r="U38" s="3" t="n">
+      <c r="U38" s="3">
         <v>19.2</v>
       </c>
-      <c r="V38" s="3" t="n">
+      <c r="V38" s="3">
         <v>20.2</v>
       </c>
-      <c r="W38" s="3" t="n">
+      <c r="W38" s="3">
         <v>21.2</v>
       </c>
-      <c r="X38" s="1" t="n">
+      <c r="X38" s="1">
         <v>22.2</v>
       </c>
-      <c r="Y38" s="1" t="n">
+      <c r="Y38" s="1">
         <v>23.2</v>
       </c>
-      <c r="Z38" s="1" t="n">
+      <c r="Z38" s="1">
         <v>24.2</v>
       </c>
-      <c r="AA38" s="3" t="n">
+      <c r="AA38" s="3">
         <v>25.2</v>
       </c>
-      <c r="AB38" s="3" t="n">
+      <c r="AB38" s="3">
         <v>26.2</v>
       </c>
-      <c r="AC38" s="3" t="n">
+      <c r="AC38" s="3">
         <v>27.2</v>
       </c>
-      <c r="AD38" s="1" t="n">
+      <c r="AD38" s="1">
         <v>28.2</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="1">
         <v>1</v>
       </c>
       <c r="C39" s="1"/>
@@ -3115,11 +3329,11 @@
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="1">
         <v>1</v>
       </c>
       <c r="C40" s="1"/>
@@ -3175,11 +3389,11 @@
       </c>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="1">
         <v>1</v>
       </c>
       <c r="C41" s="1"/>
@@ -3235,11 +3449,11 @@
       </c>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="1">
         <v>1</v>
       </c>
       <c r="C42" s="21" t="s">
@@ -3292,11 +3506,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="1" t="n">
+      <c r="B43" s="1">
         <v>1</v>
       </c>
       <c r="C43" s="7"/>
@@ -3340,11 +3554,11 @@
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="1" t="n">
+      <c r="B44" s="1">
         <v>1</v>
       </c>
       <c r="C44" s="19"/>
@@ -3386,11 +3600,11 @@
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="1" t="n">
+      <c r="B45" s="1">
         <v>1</v>
       </c>
       <c r="C45" s="1"/>
@@ -3434,11 +3648,11 @@
       <c r="AC45" s="1"/>
       <c r="AD45" s="1"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="1" t="n">
+      <c r="B46" s="1">
         <v>1</v>
       </c>
       <c r="C46" s="21" t="s">
@@ -3482,11 +3696,11 @@
       <c r="AC46" s="1"/>
       <c r="AD46" s="1"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B47" s="1" t="n">
+      <c r="B47" s="1">
         <v>1</v>
       </c>
       <c r="C47" s="1"/>
@@ -3532,11 +3746,11 @@
       <c r="AC47" s="1"/>
       <c r="AD47" s="1"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="B48" s="1">
         <v>1</v>
       </c>
       <c r="C48" s="21" t="s">
@@ -3602,11 +3816,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="1" t="n">
+      <c r="B49" s="1">
         <v>1</v>
       </c>
       <c r="C49" s="21" t="s">
@@ -3662,11 +3876,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B50" s="1" t="n">
+      <c r="B50" s="1">
         <v>1</v>
       </c>
       <c r="C50" s="21" t="s">
@@ -3712,11 +3926,11 @@
       <c r="AC50" s="1"/>
       <c r="AD50" s="1"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B51" s="1" t="n">
+      <c r="B51" s="1">
         <v>1</v>
       </c>
       <c r="C51" s="21" t="s">
@@ -3772,11 +3986,11 @@
       <c r="AC51" s="1"/>
       <c r="AD51" s="1"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="1" t="n">
+      <c r="B52" s="1">
         <v>1</v>
       </c>
       <c r="C52" s="21" t="s">
@@ -3824,11 +4038,11 @@
       </c>
       <c r="AD52" s="1"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="1" t="n">
+      <c r="B53" s="1">
         <v>1</v>
       </c>
       <c r="C53" s="21" t="s">
@@ -3874,11 +4088,11 @@
       </c>
       <c r="AD53" s="1"/>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="13" t="n">
+      <c r="B54" s="13">
         <v>1</v>
       </c>
       <c r="C54" s="13"/>
@@ -3924,11 +4138,11 @@
       </c>
       <c r="AD54" s="13"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="7" t="n">
+      <c r="B55" s="7">
         <v>2</v>
       </c>
       <c r="C55" s="7"/>
@@ -3972,11 +4186,11 @@
       <c r="AC55" s="7"/>
       <c r="AD55" s="7"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="1" t="n">
+      <c r="B56" s="1">
         <v>2</v>
       </c>
       <c r="C56" s="1"/>
@@ -4020,11 +4234,11 @@
       <c r="AC56" s="1"/>
       <c r="AD56" s="1"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="1" t="n">
+      <c r="B57" s="1">
         <v>2</v>
       </c>
       <c r="C57" s="1"/>
@@ -4068,11 +4282,11 @@
       <c r="AC57" s="1"/>
       <c r="AD57" s="1"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B58" s="1" t="n">
+      <c r="B58" s="1">
         <v>2</v>
       </c>
       <c r="C58" s="1"/>
@@ -4116,11 +4330,11 @@
       <c r="AC58" s="1"/>
       <c r="AD58" s="1"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="1" t="n">
+      <c r="B59" s="1">
         <v>2</v>
       </c>
       <c r="C59" s="1"/>
@@ -4164,11 +4378,11 @@
       <c r="AC59" s="1"/>
       <c r="AD59" s="1"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B60" s="1" t="n">
+      <c r="B60" s="1">
         <v>2</v>
       </c>
       <c r="C60" s="1"/>
@@ -4212,11 +4426,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="1" t="n">
+      <c r="B61" s="1">
         <v>2</v>
       </c>
       <c r="C61" s="19"/>
@@ -4260,11 +4474,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A62" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B62" s="1" t="n">
+      <c r="B62" s="1">
         <v>2</v>
       </c>
       <c r="C62" s="19"/>
@@ -4308,11 +4522,11 @@
       </c>
       <c r="AD62" s="1"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B63" s="1" t="n">
+      <c r="B63" s="1">
         <v>2</v>
       </c>
       <c r="C63" s="1"/>
@@ -4368,11 +4582,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A64" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B64" s="1" t="n">
+      <c r="B64" s="1">
         <v>2</v>
       </c>
       <c r="C64" s="1"/>
@@ -4416,11 +4630,11 @@
       <c r="AC64" s="1"/>
       <c r="AD64" s="1"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B65" s="1" t="n">
+      <c r="B65" s="1">
         <v>2</v>
       </c>
       <c r="C65" s="1"/>
@@ -4464,11 +4678,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B66" s="1" t="n">
+      <c r="B66" s="1">
         <v>2</v>
       </c>
       <c r="C66" s="1"/>
@@ -4524,11 +4738,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B67" s="1" t="n">
+      <c r="B67" s="1">
         <v>2</v>
       </c>
       <c r="C67" s="1"/>
@@ -4574,11 +4788,11 @@
       <c r="AC67" s="1"/>
       <c r="AD67" s="1"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B68" s="1" t="n">
+      <c r="B68" s="1">
         <v>2</v>
       </c>
       <c r="C68" s="5" t="s">
@@ -4634,11 +4848,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B69" s="1" t="n">
+      <c r="B69" s="1">
         <v>2</v>
       </c>
       <c r="C69" s="1"/>
@@ -4702,11 +4916,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B70" s="1" t="n">
+      <c r="B70" s="1">
         <v>2</v>
       </c>
       <c r="C70" s="1"/>
@@ -4762,7 +4976,7 @@
       <c r="AC70" s="1"/>
       <c r="AD70" s="1"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>49</v>
       </c>
@@ -4796,7 +5010,7 @@
       <c r="AC71" s="20"/>
       <c r="AD71" s="20"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -4886,130 +5100,122 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C73" s="3" t="n">
+      <c r="C73" s="3">
         <v>1.2</v>
       </c>
-      <c r="D73" s="3" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="E73" s="3" t="n">
+      <c r="D73" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E73" s="3">
         <v>3.2</v>
       </c>
-      <c r="F73" s="1" t="n">
+      <c r="F73" s="1">
         <v>4.2</v>
       </c>
-      <c r="G73" s="1" t="n">
+      <c r="G73" s="1">
         <v>5.2</v>
       </c>
-      <c r="H73" s="1" t="n">
+      <c r="H73" s="1">
         <v>6.2</v>
       </c>
-      <c r="I73" s="3" t="n">
+      <c r="I73" s="3">
         <v>7.2</v>
       </c>
-      <c r="J73" s="3" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="K73" s="3" t="n">
-        <v>9.2</v>
-      </c>
-      <c r="L73" s="1" t="n">
-        <v>10.2</v>
-      </c>
-      <c r="M73" s="1" t="n">
+      <c r="J73" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K73" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L73" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M73" s="1">
         <v>11.2</v>
       </c>
-      <c r="N73" s="1" t="n">
+      <c r="N73" s="1">
         <v>12.2</v>
       </c>
-      <c r="O73" s="3" t="n">
+      <c r="O73" s="3">
         <v>13.2</v>
       </c>
-      <c r="P73" s="3" t="n">
+      <c r="P73" s="3">
         <v>14.2</v>
       </c>
-      <c r="Q73" s="3" t="n">
+      <c r="Q73" s="3">
         <v>15.2</v>
       </c>
-      <c r="R73" s="1" t="n">
+      <c r="R73" s="1">
         <v>16.2</v>
       </c>
-      <c r="S73" s="1" t="n">
+      <c r="S73" s="1">
         <v>17.2</v>
       </c>
-      <c r="T73" s="1" t="n">
+      <c r="T73" s="1">
         <v>18.2</v>
       </c>
-      <c r="U73" s="3" t="n">
+      <c r="U73" s="3">
         <v>19.2</v>
       </c>
-      <c r="V73" s="3" t="n">
+      <c r="V73" s="3">
         <v>20.2</v>
       </c>
-      <c r="W73" s="3" t="n">
+      <c r="W73" s="3">
         <v>21.2</v>
       </c>
-      <c r="X73" s="1" t="n">
+      <c r="X73" s="1">
         <v>22.2</v>
       </c>
-      <c r="Y73" s="1" t="n">
+      <c r="Y73" s="1">
         <v>23.2</v>
       </c>
-      <c r="Z73" s="1" t="n">
+      <c r="Z73" s="1">
         <v>24.2</v>
       </c>
-      <c r="AA73" s="3" t="n">
+      <c r="AA73" s="3">
         <v>25.2</v>
       </c>
-      <c r="AB73" s="3" t="n">
+      <c r="AB73" s="3">
         <v>26.2</v>
       </c>
-      <c r="AC73" s="3" t="n">
+      <c r="AC73" s="3">
         <v>27.2</v>
       </c>
-      <c r="AD73" s="1" t="n">
+      <c r="AD73" s="1">
         <v>28.2</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D44:E44">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C25 C14:C15 C44 C3 C6 C8:C12">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.14"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5099,101 +5305,101 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="3">
         <v>1.2</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="E2" s="3" t="n">
+      <c r="D2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E2" s="3">
         <v>3.2</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="1">
         <v>4.2</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="1">
         <v>5.2</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>6.2</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="3">
         <v>7.2</v>
       </c>
-      <c r="J2" s="3" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="K2" s="3" t="n">
-        <v>9.2</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>10.2</v>
-      </c>
-      <c r="M2" s="1" t="n">
+      <c r="J2" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K2" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M2" s="1">
         <v>11.2</v>
       </c>
-      <c r="N2" s="1" t="n">
+      <c r="N2" s="1">
         <v>12.2</v>
       </c>
-      <c r="O2" s="3" t="n">
+      <c r="O2" s="3">
         <v>13.2</v>
       </c>
-      <c r="P2" s="3" t="n">
+      <c r="P2" s="3">
         <v>14.2</v>
       </c>
-      <c r="Q2" s="3" t="n">
+      <c r="Q2" s="3">
         <v>15.2</v>
       </c>
-      <c r="R2" s="1" t="n">
+      <c r="R2" s="1">
         <v>16.2</v>
       </c>
-      <c r="S2" s="1" t="n">
+      <c r="S2" s="1">
         <v>17.2</v>
       </c>
-      <c r="T2" s="1" t="n">
+      <c r="T2" s="1">
         <v>18.2</v>
       </c>
-      <c r="U2" s="3" t="n">
+      <c r="U2" s="3">
         <v>19.2</v>
       </c>
-      <c r="V2" s="3" t="n">
+      <c r="V2" s="3">
         <v>20.2</v>
       </c>
-      <c r="W2" s="3" t="n">
+      <c r="W2" s="3">
         <v>21.2</v>
       </c>
-      <c r="X2" s="1" t="n">
+      <c r="X2" s="1">
         <v>22.2</v>
       </c>
-      <c r="Y2" s="1" t="n">
+      <c r="Y2" s="1">
         <v>23.2</v>
       </c>
-      <c r="Z2" s="1" t="n">
+      <c r="Z2" s="1">
         <v>24.2</v>
       </c>
-      <c r="AA2" s="3" t="n">
+      <c r="AA2" s="3">
         <v>25.2</v>
       </c>
-      <c r="AB2" s="3" t="n">
+      <c r="AB2" s="3">
         <v>26.2</v>
       </c>
-      <c r="AC2" s="3" t="n">
+      <c r="AC2" s="3">
         <v>27.2</v>
       </c>
-      <c r="AD2" s="1" t="n">
+      <c r="AD2" s="1">
         <v>28.2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -5251,11 +5457,11 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
@@ -5303,11 +5509,11 @@
       </c>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1"/>
@@ -5353,11 +5559,11 @@
       </c>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -5403,11 +5609,11 @@
       </c>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -5453,11 +5659,11 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -5513,11 +5719,11 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -5573,11 +5779,11 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="8"/>
@@ -5623,11 +5829,11 @@
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -5685,11 +5891,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -5737,11 +5943,11 @@
       </c>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1"/>
@@ -5789,11 +5995,11 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -5857,11 +6063,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -5909,11 +6115,11 @@
       </c>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1"/>
@@ -5959,11 +6165,11 @@
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="10" t="n">
+      <c r="B17" s="10">
         <v>1</v>
       </c>
       <c r="C17" s="11"/>
@@ -6007,11 +6213,11 @@
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="10" t="n">
+      <c r="B18" s="10">
         <v>1</v>
       </c>
       <c r="C18" s="11"/>
@@ -6055,11 +6261,11 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="13" t="n">
+      <c r="B19" s="13">
         <v>1</v>
       </c>
       <c r="C19" s="13"/>
@@ -6123,11 +6329,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="17" t="s">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="7" t="n">
+      <c r="B20" s="7">
         <v>2</v>
       </c>
       <c r="C20" s="7"/>
@@ -6171,11 +6377,11 @@
       <c r="AC20" s="7"/>
       <c r="AD20" s="7"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="1">
         <v>2</v>
       </c>
       <c r="C21" s="8"/>
@@ -6219,11 +6425,11 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="1">
         <v>2</v>
       </c>
       <c r="C22" s="8"/>
@@ -6279,11 +6485,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="B23" s="1">
         <v>2</v>
       </c>
       <c r="C23" s="8"/>
@@ -6327,11 +6533,11 @@
       <c r="AC23" s="7"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" s="1">
         <v>2</v>
       </c>
       <c r="C24" s="19"/>
@@ -6375,11 +6581,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="8"/>
@@ -6425,11 +6631,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" s="1">
         <v>2</v>
       </c>
       <c r="C26" s="1"/>
@@ -6485,11 +6691,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="1">
         <v>2</v>
       </c>
       <c r="C27" s="1"/>
@@ -6535,11 +6741,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="1">
         <v>2</v>
       </c>
       <c r="C28" s="1"/>
@@ -6585,11 +6791,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="1">
         <v>2</v>
       </c>
       <c r="C29" s="1"/>
@@ -6635,11 +6841,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="1">
         <v>2</v>
       </c>
       <c r="C30" s="1"/>
@@ -6695,11 +6901,11 @@
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="1">
         <v>2</v>
       </c>
       <c r="C31" s="1"/>
@@ -6765,11 +6971,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="1">
         <v>2</v>
       </c>
       <c r="C32" s="1"/>
@@ -6815,11 +7021,11 @@
       </c>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="1">
         <v>2</v>
       </c>
       <c r="C33" s="1"/>
@@ -6875,11 +7081,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="1">
         <v>2</v>
       </c>
       <c r="C34" s="1"/>
@@ -6923,11 +7129,11 @@
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="1">
         <v>2</v>
       </c>
       <c r="C35" s="1"/>
@@ -6993,11 +7199,11 @@
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="1" t="n">
+      <c r="B36" s="1">
         <v>1</v>
       </c>
       <c r="C36" s="1"/>
@@ -7043,11 +7249,11 @@
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="1">
         <v>1</v>
       </c>
       <c r="C37" s="1"/>
@@ -7103,11 +7309,11 @@
       </c>
       <c r="AD37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="1">
         <v>1</v>
       </c>
       <c r="C38" s="1"/>
@@ -7163,11 +7369,11 @@
       </c>
       <c r="AD38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="1">
         <v>1</v>
       </c>
       <c r="C39" s="21" t="s">
@@ -7220,11 +7426,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="1">
         <v>1</v>
       </c>
       <c r="C40" s="7"/>
@@ -7268,11 +7474,11 @@
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="21" t="s">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="1">
         <v>1</v>
       </c>
       <c r="C41" s="19"/>
@@ -7314,11 +7520,11 @@
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="21" t="s">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="1">
         <v>1</v>
       </c>
       <c r="C42" s="1"/>
@@ -7362,11 +7568,11 @@
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="21" t="s">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="1" t="n">
+      <c r="B43" s="1">
         <v>1</v>
       </c>
       <c r="C43" s="21" t="s">
@@ -7410,11 +7616,11 @@
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="21" t="s">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B44" s="1" t="n">
+      <c r="B44" s="1">
         <v>1</v>
       </c>
       <c r="C44" s="1"/>
@@ -7460,11 +7666,11 @@
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="21" t="s">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A45" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="1" t="n">
+      <c r="B45" s="1">
         <v>1</v>
       </c>
       <c r="C45" s="21" t="s">
@@ -7530,11 +7736,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="21" t="s">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A46" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B46" s="1" t="n">
+      <c r="B46" s="1">
         <v>1</v>
       </c>
       <c r="C46" s="21" t="s">
@@ -7590,11 +7796,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="21" t="s">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A47" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="1" t="n">
+      <c r="B47" s="1">
         <v>1</v>
       </c>
       <c r="C47" s="21" t="s">
@@ -7640,11 +7846,11 @@
       <c r="AC47" s="1"/>
       <c r="AD47" s="1"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="21" t="s">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A48" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="B48" s="1">
         <v>1</v>
       </c>
       <c r="C48" s="21" t="s">
@@ -7700,11 +7906,11 @@
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="21" t="s">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="1" t="n">
+      <c r="B49" s="1">
         <v>1</v>
       </c>
       <c r="C49" s="21" t="s">
@@ -7752,11 +7958,11 @@
       </c>
       <c r="AD49" s="1"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="21" t="s">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="1" t="n">
+      <c r="B50" s="1">
         <v>1</v>
       </c>
       <c r="C50" s="21" t="s">
@@ -7802,11 +8008,11 @@
       </c>
       <c r="AD50" s="1"/>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="22" t="s">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A51" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="13" t="n">
+      <c r="B51" s="13">
         <v>1</v>
       </c>
       <c r="C51" s="13"/>
@@ -7852,11 +8058,11 @@
       </c>
       <c r="AD51" s="13"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="24" t="s">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A52" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="7" t="n">
+      <c r="B52" s="7">
         <v>2</v>
       </c>
       <c r="C52" s="7"/>
@@ -7900,11 +8106,11 @@
       <c r="AC52" s="7"/>
       <c r="AD52" s="7"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="21" t="s">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A53" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B53" s="1" t="n">
+      <c r="B53" s="1">
         <v>2</v>
       </c>
       <c r="C53" s="1"/>
@@ -7948,11 +8154,11 @@
       <c r="AC53" s="1"/>
       <c r="AD53" s="1"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="21" t="s">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A54" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B54" s="1" t="n">
+      <c r="B54" s="1">
         <v>2</v>
       </c>
       <c r="C54" s="1"/>
@@ -7996,11 +8202,11 @@
       <c r="AC54" s="1"/>
       <c r="AD54" s="1"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="21" t="s">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A55" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="1" t="n">
+      <c r="B55" s="1">
         <v>2</v>
       </c>
       <c r="C55" s="1"/>
@@ -8044,11 +8250,11 @@
       <c r="AC55" s="1"/>
       <c r="AD55" s="1"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="21" t="s">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A56" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B56" s="1" t="n">
+      <c r="B56" s="1">
         <v>2</v>
       </c>
       <c r="C56" s="1"/>
@@ -8092,11 +8298,11 @@
       <c r="AC56" s="1"/>
       <c r="AD56" s="1"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="21" t="s">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A57" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="1" t="n">
+      <c r="B57" s="1">
         <v>2</v>
       </c>
       <c r="C57" s="1"/>
@@ -8140,11 +8346,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="21" t="s">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A58" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B58" s="1" t="n">
+      <c r="B58" s="1">
         <v>2</v>
       </c>
       <c r="C58" s="19"/>
@@ -8188,11 +8394,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="21" t="s">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A59" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B59" s="1" t="n">
+      <c r="B59" s="1">
         <v>2</v>
       </c>
       <c r="C59" s="19"/>
@@ -8236,11 +8442,11 @@
       </c>
       <c r="AD59" s="1"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="21" t="s">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A60" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B60" s="1" t="n">
+      <c r="B60" s="1">
         <v>2</v>
       </c>
       <c r="C60" s="1"/>
@@ -8296,11 +8502,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="21" t="s">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A61" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="1" t="n">
+      <c r="B61" s="1">
         <v>2</v>
       </c>
       <c r="C61" s="1"/>
@@ -8344,11 +8550,11 @@
       <c r="AC61" s="1"/>
       <c r="AD61" s="1"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="21" t="s">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A62" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B62" s="1" t="n">
+      <c r="B62" s="1">
         <v>2</v>
       </c>
       <c r="C62" s="1"/>
@@ -8392,11 +8598,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="21" t="s">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A63" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B63" s="1" t="n">
+      <c r="B63" s="1">
         <v>2</v>
       </c>
       <c r="C63" s="1"/>
@@ -8452,11 +8658,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="21" t="s">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A64" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B64" s="1" t="n">
+      <c r="B64" s="1">
         <v>2</v>
       </c>
       <c r="C64" s="1"/>
@@ -8502,11 +8708,11 @@
       <c r="AC64" s="1"/>
       <c r="AD64" s="1"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="21" t="s">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A65" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B65" s="1" t="n">
+      <c r="B65" s="1">
         <v>2</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -8562,11 +8768,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="21" t="s">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A66" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B66" s="1" t="n">
+      <c r="B66" s="1">
         <v>2</v>
       </c>
       <c r="C66" s="1"/>
@@ -8630,11 +8836,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="21" t="s">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A67" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B67" s="1" t="n">
+      <c r="B67" s="1">
         <v>2</v>
       </c>
       <c r="C67" s="1"/>
@@ -8692,347 +8898,334 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D41:E41">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41 C17:C25 C14:C15 C3 C6 C8:C12">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.29"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>146</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="aarutinovi@evolution.com "/>
+    <hyperlink ref="A4" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>